<commit_message>
Refactoring para permitir células não mapeadas nas entidades
</commit_message>
<xml_diff>
--- a/src/test/resources/marxls/Pasta2.xlsx
+++ b/src/test/resources/marxls/Pasta2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>D02</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>tag3</t>
+  </si>
+  <si>
+    <t>teste1</t>
+  </si>
+  <si>
+    <t>teste2</t>
+  </si>
+  <si>
+    <t>C05</t>
   </si>
   <si>
     <t>teste 1;teste 2</t>
@@ -431,7 +440,7 @@
   <dimension ref="A4:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +493,7 @@
         <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -537,15 +546,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:E4"/>
+  <dimension ref="C2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -555,8 +564,11 @@
       <c r="E2" t="s">
         <v>15</v>
       </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>11</v>
       </c>
@@ -566,8 +578,11 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -576,6 +591,9 @@
       </c>
       <c r="E4" t="s">
         <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>